<commit_message>
começo do caso de uso 1.0
</commit_message>
<xml_diff>
--- a/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
+++ b/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Atores" sheetId="2" r:id="rId2"/>
+    <sheet name="UC 1.0" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -256,13 +256,46 @@
   </si>
   <si>
     <t>Representa as pessoas que utilizarão o sistema em suas funções mais avançadas</t>
+  </si>
+  <si>
+    <t>Fluxo Principal</t>
+  </si>
+  <si>
+    <t>Atores envolvidos</t>
+  </si>
+  <si>
+    <t>Pré condições</t>
+  </si>
+  <si>
+    <t>Fluxo Alternativo</t>
+  </si>
+  <si>
+    <t>Regras de negócio</t>
+  </si>
+  <si>
+    <t>Pós-condições</t>
+  </si>
+  <si>
+    <t>Casos de Uso</t>
+  </si>
+  <si>
+    <t>Funcionário e Administrador</t>
+  </si>
+  <si>
+    <t>PR1 - O Funcionário ou Administrador devem estar na tela cadastro de clientes</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador devem preencher os campos do formulário(nome, login, senha, cpf,endereço, telefone, e-mail, conta bancária)</t>
+  </si>
+  <si>
+    <t>AF1 - Se houver algum formulário não preenchido ou com erro no preenchimento aparecerá uma mensagem de erro na tela pedindo para que o funcionário ou administrador a preencha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,8 +333,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,8 +361,20 @@
         <bgColor rgb="FFB7B7B7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -329,12 +382,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,6 +417,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1152,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1164,7 +1237,7 @@
     <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>74</v>
       </c>
@@ -1172,7 +1245,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="141" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>76</v>
       </c>
@@ -1180,7 +1253,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="141" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>78</v>
       </c>
@@ -1199,12 +1272,81 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="164.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Caso de uso 1.0 pronto
</commit_message>
<xml_diff>
--- a/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
+++ b/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Descrição</t>
   </si>
   <si>
-    <t>Usuário</t>
-  </si>
-  <si>
     <t>Representa as pessoas que utilizarão o sistema em suas funções básicas de operação</t>
   </si>
   <si>
@@ -282,20 +279,47 @@
     <t>Funcionário e Administrador</t>
   </si>
   <si>
-    <t>PR1 - O Funcionário ou Administrador devem estar na tela cadastro de clientes</t>
-  </si>
-  <si>
-    <t>FP1 - O Funcionário ou Administrador devem preencher os campos do formulário(nome, login, senha, cpf,endereço, telefone, e-mail, conta bancária)</t>
-  </si>
-  <si>
-    <t>AF1 - Se houver algum formulário não preenchido ou com erro no preenchimento aparecerá uma mensagem de erro na tela pedindo para que o funcionário ou administrador a preencha</t>
+    <t>AF1 - Se houver algum formulário não preenchido ou com erro no preenchimento aparecerá uma mensagem de erro na tela pedindo para que o funcionário ou administrador a preencha corretamente.</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador devem preencher os campos do formulário(nome, cpf,endereço, telefone, e-mail)</t>
+  </si>
+  <si>
+    <t>O cliente estará cadastrado</t>
+  </si>
+  <si>
+    <t>RN1 - O nome deve ter no mínimo 5 e no máximo 40 caracteres;</t>
+  </si>
+  <si>
+    <t>RN2 - O cpf deverá receber somente números e no máximo 11 caracteres;</t>
+  </si>
+  <si>
+    <t>RN3 - O endereço deverá ter no mínimo 5 e no máximo 50 caracteres;</t>
+  </si>
+  <si>
+    <t>RN4 - O telefone deverá ter somente números e no mínimo 9 caracteres e no máximo 15;</t>
+  </si>
+  <si>
+    <t>RN5 - O e-mail deverá ter no mínimo 5 caracteres e no máximo 50, além de ter que possuir um "@".</t>
+  </si>
+  <si>
+    <t>PR1 - O Funcionário ou Administrador devem ter logados no sistema;</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador devem estar na tela cadastro de clientes.</t>
+  </si>
+  <si>
+    <t>UC 1.1, UC 1.2, UC 1.3</t>
+  </si>
+  <si>
+    <t>Funcionário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +365,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -374,7 +403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -397,12 +426,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,7 +538,20 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1225,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,19 +1376,19 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>78</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1272,16 +1402,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="164.28515625" customWidth="1"/>
+    <col min="3" max="3" width="176.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1293,57 +1423,93 @@
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C4" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="8" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="C12" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
+      <c r="C14" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Caso de uso 1.1 pronto
</commit_message>
<xml_diff>
--- a/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
+++ b/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Atores" sheetId="2" r:id="rId2"/>
     <sheet name="UC 1.0" sheetId="3" r:id="rId3"/>
+    <sheet name="UC 1.1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="106">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -132,9 +133,6 @@
     <t>Cadastrar Cliente</t>
   </si>
   <si>
-    <t>Listar Cliente</t>
-  </si>
-  <si>
     <t>Alterar dados do Cliente</t>
   </si>
   <si>
@@ -313,6 +311,30 @@
   </si>
   <si>
     <t>Funcionário</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Listar Clientes</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador devem estar na tela cadastro de busca de clientes.</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador devem preencher o campo do formulário para pesquisa</t>
+  </si>
+  <si>
+    <t>AF1 - Se não houver nenhum cliete com alguma ligação com o que foi pesquisado o sistema retornará uma mensagem.</t>
+  </si>
+  <si>
+    <t>Aparecerá uma lista com os clientes com o que foi descrito na pesquisa</t>
+  </si>
+  <si>
+    <t>UC 1.2, UC 1.3</t>
+  </si>
+  <si>
+    <t>RN1 - O funcionário ou administrador deverá clicar no botão "pesquisar"</t>
   </si>
 </sst>
 </file>
@@ -857,7 +879,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,10 +912,10 @@
         <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -901,13 +923,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,13 +937,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -929,13 +951,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -943,13 +965,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -957,13 +979,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -971,13 +993,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -985,13 +1007,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -999,13 +1021,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1013,13 +1035,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,13 +1049,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1041,13 +1063,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1055,13 +1077,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" s="3"/>
     </row>
@@ -1070,13 +1092,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1084,13 +1106,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,13 +1120,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1112,13 +1134,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,13 +1148,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1140,13 +1162,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1154,13 +1176,13 @@
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,13 +1190,13 @@
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1182,13 +1204,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,13 +1218,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,13 +1232,13 @@
         <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,13 +1246,13 @@
         <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1238,13 +1260,13 @@
         <v>29</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,13 +1274,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,13 +1288,13 @@
         <v>31</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,13 +1302,13 @@
         <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,13 +1316,13 @@
         <v>33</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1308,13 +1330,13 @@
         <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1322,13 +1344,13 @@
         <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,13 +1358,13 @@
         <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1355,7 +1377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1369,26 +1391,26 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>77</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1405,7 +1427,7 @@
   <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B2" sqref="B2:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,88 +1446,88 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -1515,4 +1537,93 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="176.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Casos de uso 1.3 e 3.0 prontos
</commit_message>
<xml_diff>
--- a/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
+++ b/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
@@ -4,20 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Atores" sheetId="2" r:id="rId2"/>
     <sheet name="UC 1.0" sheetId="3" r:id="rId3"/>
     <sheet name="UC 1.1" sheetId="4" r:id="rId4"/>
+    <sheet name="UC 1.2" sheetId="5" r:id="rId5"/>
+    <sheet name="UC 1.3" sheetId="6" r:id="rId6"/>
+    <sheet name="UC 2.0" sheetId="8" r:id="rId7"/>
+    <sheet name="UC 2.1" sheetId="9" r:id="rId8"/>
+    <sheet name="UC 2.2" sheetId="10" r:id="rId9"/>
+    <sheet name="UC 3.0" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="129">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -280,9 +286,6 @@
     <t>AF1 - Se houver algum formulário não preenchido ou com erro no preenchimento aparecerá uma mensagem de erro na tela pedindo para que o funcionário ou administrador a preencha corretamente.</t>
   </si>
   <si>
-    <t>FP1 - O Funcionário ou Administrador devem preencher os campos do formulário(nome, cpf,endereço, telefone, e-mail)</t>
-  </si>
-  <si>
     <t>O cliente estará cadastrado</t>
   </si>
   <si>
@@ -301,12 +304,6 @@
     <t>RN5 - O e-mail deverá ter no mínimo 5 caracteres e no máximo 50, além de ter que possuir um "@".</t>
   </si>
   <si>
-    <t>PR1 - O Funcionário ou Administrador devem ter logados no sistema;</t>
-  </si>
-  <si>
-    <t>PR2 - O Funcionário ou Administrador devem estar na tela cadastro de clientes.</t>
-  </si>
-  <si>
     <t>UC 1.1, UC 1.2, UC 1.3</t>
   </si>
   <si>
@@ -319,12 +316,6 @@
     <t>Listar Clientes</t>
   </si>
   <si>
-    <t>PR2 - O Funcionário ou Administrador devem estar na tela cadastro de busca de clientes.</t>
-  </si>
-  <si>
-    <t>FP1 - O Funcionário ou Administrador devem preencher o campo do formulário para pesquisa</t>
-  </si>
-  <si>
     <t>AF1 - Se não houver nenhum cliete com alguma ligação com o que foi pesquisado o sistema retornará uma mensagem.</t>
   </si>
   <si>
@@ -335,6 +326,90 @@
   </si>
   <si>
     <t>RN1 - O funcionário ou administrador deverá clicar no botão "pesquisar"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alterar dados do cliente </t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador deve estar na tela cadastro de busca de clientes.</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador deve preencher o campo do formulário para pesquisa</t>
+  </si>
+  <si>
+    <t>FP2 - O Funcionário ou Administrador deve clicar em "confirmar alterações".</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador deve preencher o campo do formulário na qual deseje alterar(nome,cpf,endereço, e-mail, telefone);</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador deve estar na tela cadastro de busca de clientes;</t>
+  </si>
+  <si>
+    <t>PR3 - O Funcionário ou Administrador deve ter selecionado o cliente e clicar em "editar dados".</t>
+  </si>
+  <si>
+    <t>PR1 - O Funcionário ou Administrador deve ter logado no sistema;</t>
+  </si>
+  <si>
+    <t>AF1 - Se os dados preenchidos não forem condizentes com o tipo de dado requerido aparecerá uma mensagem de erro</t>
+  </si>
+  <si>
+    <t>UC 1.0, UC 1.1, UC 1.3</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador deve estar na tela cadastro de clientes.</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador deve preencher os campos do formulário(nome, cpf,endereço, telefone, e-mail)</t>
+  </si>
+  <si>
+    <t>PR3 - O Funcionário ou Administrador deve ter selecionado o cliente no qual quer remover.</t>
+  </si>
+  <si>
+    <t>AF1 - Caso não queira remover o cliente, o Funcionário ou Administrador deverá clicar em "não"</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador deve clicar em "Remover Cliente";</t>
+  </si>
+  <si>
+    <t>FP2 - Aparecerá uma mensagem de confirção, o Funcionário ou Administrador deve clicar em "sim".</t>
+  </si>
+  <si>
+    <t>Os dados do Cliente terão alterado</t>
+  </si>
+  <si>
+    <t>O cliente terá sido excluído</t>
+  </si>
+  <si>
+    <t>Abrir Caixa</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador deve estar na tela cadastro de insumos.</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador deve preencher os campos do formulário(descrição, quantidade, validade, fabricação, fornecedor);</t>
+  </si>
+  <si>
+    <t>FP2 - O Funcionário ou Administrador deve clicar em "Confirmar".</t>
+  </si>
+  <si>
+    <t>RN1 - A descrição deve ter no mínimo 5 e no máximo 40 caracteres;</t>
+  </si>
+  <si>
+    <t>RN2 - A validade e fabricação deverão receber valores no formato de data "dd/mm/aaa";</t>
+  </si>
+  <si>
+    <t>RN4 - O fornecedor deverá receber o código do fornecedor cadastrado no sistema.</t>
+  </si>
+  <si>
+    <t>RN3 - O quantidade deverá receber números inteiros;</t>
+  </si>
+  <si>
+    <t>UC 3.1, UC 3.2, UC 3.3</t>
+  </si>
+  <si>
+    <t>O Insumo estará cadastrado</t>
   </si>
 </sst>
 </file>
@@ -425,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -536,12 +611,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -574,6 +660,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,7 +969,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +1005,7 @@
         <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -923,7 +1013,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>70</v>
@@ -1370,6 +1460,119 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="176.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -1399,7 +1602,7 @@
     </row>
     <row r="4" spans="2:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>75</v>
@@ -1426,7 +1629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C14"/>
     </sheetView>
   </sheetViews>
@@ -1457,13 +1660,13 @@
         <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="20" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1471,7 +1674,7 @@
         <v>78</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1487,31 +1690,31 @@
         <v>82</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="13"/>
       <c r="C12" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -1519,7 +1722,7 @@
         <v>83</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
@@ -1527,7 +1730,7 @@
         <v>84</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
@@ -1543,14 +1746,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="176.7109375" customWidth="1"/>
+    <col min="3" max="3" width="112" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
@@ -1558,7 +1761,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1574,13 +1777,13 @@
         <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="20" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1588,7 +1791,7 @@
         <v>78</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1596,7 +1799,7 @@
         <v>81</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1604,7 +1807,7 @@
         <v>82</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1612,7 +1815,7 @@
         <v>83</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -1620,10 +1823,315 @@
         <v>84</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="124" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="123.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="88.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="22"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
use case 3.1 pronto
</commit_message>
<xml_diff>
--- a/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
+++ b/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evanio\Desktop\SistemaGestaoPecuaria\Documentos\Documentação de Caso de Uso\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -17,13 +22,14 @@
     <sheet name="UC 2.1" sheetId="9" r:id="rId8"/>
     <sheet name="UC 2.2" sheetId="10" r:id="rId9"/>
     <sheet name="UC 3.0" sheetId="11" r:id="rId10"/>
+    <sheet name="UC 3.1" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="132">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -316,12 +322,6 @@
     <t>Listar Clientes</t>
   </si>
   <si>
-    <t>AF1 - Se não houver nenhum cliete com alguma ligação com o que foi pesquisado o sistema retornará uma mensagem.</t>
-  </si>
-  <si>
-    <t>Aparecerá uma lista com os clientes com o que foi descrito na pesquisa</t>
-  </si>
-  <si>
     <t>UC 1.2, UC 1.3</t>
   </si>
   <si>
@@ -331,9 +331,6 @@
     <t xml:space="preserve">Alterar dados do cliente </t>
   </si>
   <si>
-    <t>PR2 - O Funcionário ou Administrador deve estar na tela cadastro de busca de clientes.</t>
-  </si>
-  <si>
     <t>FP1 - O Funcionário ou Administrador deve preencher o campo do formulário para pesquisa</t>
   </si>
   <si>
@@ -410,6 +407,24 @@
   </si>
   <si>
     <t>O Insumo estará cadastrado</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador deve estar na tela de busca de clientes.</t>
+  </si>
+  <si>
+    <t>AF1 - Se não houver nenhum cliete com alguma ligação com o que foi pesquisado o sistema retornará uma mensagemde erro;</t>
+  </si>
+  <si>
+    <t>Aparecerá uma lista com os clientes com o que foram descritos na pesquisa</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador deve estar na tela de busca de insumos.</t>
+  </si>
+  <si>
+    <t>AF1 - Se não houver nenhum Insumo com alguma ligação com o que foi pesquisado o sistema retornará uma mensagemde erro;</t>
+  </si>
+  <si>
+    <t>Aparecerá uma lista com os Insumos  que foram descritos na pesquisa</t>
   </si>
 </sst>
 </file>
@@ -675,6 +690,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -722,7 +740,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -757,7 +775,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -969,7 +987,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C14" sqref="B2:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,13 +1516,13 @@
         <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1512,13 +1530,13 @@
         <v>78</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
       <c r="C7" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1534,25 +1552,25 @@
         <v>82</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
       <c r="C12" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
@@ -1560,7 +1578,7 @@
         <v>83</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
@@ -1568,7 +1586,96 @@
         <v>84</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="113.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="20" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1630,7 +1737,7 @@
   <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,13 +1767,13 @@
         <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1674,7 +1781,7 @@
         <v>78</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1747,7 +1854,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,13 +1884,13 @@
         <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="20" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1791,7 +1898,7 @@
         <v>78</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1799,7 +1906,7 @@
         <v>81</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
@@ -1807,7 +1914,7 @@
         <v>82</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1815,7 +1922,7 @@
         <v>83</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -1823,7 +1930,7 @@
         <v>84</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1850,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1866,19 +1973,19 @@
         <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1886,13 +1993,13 @@
         <v>78</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1900,7 +2007,7 @@
         <v>81</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -1914,7 +2021,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -1922,7 +2029,7 @@
         <v>84</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1949,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -1965,19 +2072,19 @@
         <v>80</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -1985,13 +2092,13 @@
         <v>78</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -1999,7 +2106,7 @@
         <v>81</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
@@ -2013,7 +2120,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
@@ -2021,7 +2128,7 @@
         <v>84</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2048,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
use case 3.2 pronto
</commit_message>
<xml_diff>
--- a/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
+++ b/Documentos/Documentação de Caso de Uso/Documentação de caso de uso.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="UC 2.2" sheetId="10" r:id="rId9"/>
     <sheet name="UC 3.0" sheetId="11" r:id="rId10"/>
     <sheet name="UC 3.1" sheetId="13" r:id="rId11"/>
+    <sheet name="UC 3.2" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="138">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -425,6 +426,24 @@
   </si>
   <si>
     <t>Aparecerá uma lista com os Insumos  que foram descritos na pesquisa</t>
+  </si>
+  <si>
+    <t>Alterar dados do Insumo</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador deve estar na tela de busca de clientes;</t>
+  </si>
+  <si>
+    <t>PR2 - O Funcionário ou Administrador deve estar na tela de busca de Insumos ;</t>
+  </si>
+  <si>
+    <t>PR3 - O Funcionário ou Administrador deve ter selecionado o Insumo e clicar em "editar dados".</t>
+  </si>
+  <si>
+    <t>FP1 - O Funcionário ou Administrador deve preencher o campo do formulário na qual deseje alterar(descrição, quantidade, validade, fabricação, fornecedor);</t>
+  </si>
+  <si>
+    <t>Os dados do Insumo terão alterado</t>
   </si>
 </sst>
 </file>
@@ -515,7 +534,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -637,12 +656,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -679,6 +724,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1486,7 +1533,7 @@
   <dimension ref="B2:C14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C14" sqref="B2:C14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,7 +1645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1676,6 +1723,101 @@
       </c>
       <c r="C10" s="8" t="s">
         <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="139.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1943,7 +2085,7 @@
   <dimension ref="B2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,7 +2121,7 @@
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="22" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>